<commit_message>
Add seed data and fix manual light theme headers
- Regenerate seed_assets.xlsx with 50 random assets using valid IRS property classes
- Fix manual headers not displaying correctly in light theme by adding prose-headings:text-foreground

🤖 Generated with [Claude Code](https://claude.com/claude-code)
</commit_message>
<xml_diff>
--- a/seed_assets.xlsx
+++ b/seed_assets.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Assets" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,24 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-    <col width="40" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -485,545 +471,529 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dell OptiPlex 7090</t>
+          <t>Reception Desk #5475</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Desktop workstation, Intel i7, 32GB RAM, 512GB SSD</t>
+          <t>L-shaped reception counter</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1450</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>100</v>
+          <t>2019-10-19</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>835.53</v>
+      </c>
+      <c r="F2" t="n">
+        <v>96.44</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>IT Department - Workstation #12</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HP LaserJet Pro M454dw</t>
+          <t>Lathe #2876</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Color laser printer for marketing department</t>
+          <t>Industrial metal lathe</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Machinery</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>549.99</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>50</v>
+          <t>2022-05-07</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>83433.28</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9217.5</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>5-year property</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Marketing floor printer</t>
-        </is>
-      </c>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MacBook Pro 16"</t>
+          <t>Printer #9197</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M2 Max, 64GB RAM, 1TB SSD - Developer laptop</t>
+          <t>HP LaserJet multifunction printer</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-02-10</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>3499</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>200</v>
+          <t>2024-08-22</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3137.6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>293.2</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>5-year property</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Assigned to senior developer</t>
-        </is>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cisco IP Phone 8845</t>
+          <t>Pickup Truck #3295</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VoIP desk phone with video capability</t>
+          <t>Ford F-150 pickup</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-06-20</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>389</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>25</v>
+          <t>2021-07-08</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>21523.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2197.91</v>
       </c>
       <c r="G5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Executive office</t>
+          <t>Refurbished</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Epson SureColor P900</t>
+          <t>Conference Table #2965</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17-inch professional photo printer</t>
+          <t>10-seat conference room table</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023-08-05</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>1295</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>100</v>
+          <t>2019-04-17</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2111.79</v>
+      </c>
+      <c r="F6" t="n">
+        <v>288.77</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Design studio</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Herman Miller Aeron Chair</t>
+          <t>Backup Generator #4366</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ergonomic office chair, size B, graphite</t>
+          <t>Diesel backup generator</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Building Equipment</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023-04-12</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>1395</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>150</v>
+          <t>2024-06-07</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>43425.48</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5835.69</v>
       </c>
       <c r="G7" t="n">
         <v>10</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>CEO office</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Standing Desk - Uplift V2</t>
+          <t>Pickup Truck #1846</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>72" commercial grade standing desk</t>
+          <t>Ford F-150 pickup</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023-05-01</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>899</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>75</v>
+          <t>2020-12-15</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>43305.29</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3841.12</v>
       </c>
       <c r="G8" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>7-year property</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Engineering workspace</t>
-        </is>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Conference Table</t>
+          <t>Ergonomic Chair #8269</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12-person mahogany conference table</t>
+          <t>Herman Miller Aeron chair</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2021-09-15</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>4500</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>400</v>
+          <t>2016-08-21</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2802.24</v>
+      </c>
+      <c r="F9" t="n">
+        <v>171.19</v>
       </c>
       <c r="G9" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Main boardroom</t>
+          <t>Needs maintenance</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Filing Cabinet System</t>
+          <t>Bookshelf #6337</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4-drawer lateral file cabinet, fireproof</t>
+          <t>6-shelf office bookcase</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-01-08</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>100</v>
+          <t>2025-04-28</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1875.69</v>
+      </c>
+      <c r="F10" t="n">
+        <v>254.1</v>
       </c>
       <c r="G10" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7-year property</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>HR document storage</t>
-        </is>
-      </c>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Reception Desk</t>
+          <t>Dell Laptop #3226</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Custom L-shaped reception desk with granite top</t>
+          <t>Dell Latitude laptop computer</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2020-03-20</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>3200</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>300</v>
+          <t>2024-11-11</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2173.64</v>
+      </c>
+      <c r="F11" t="n">
+        <v>163.77</v>
       </c>
       <c r="G11" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Main lobby</t>
+          <t>Extended warranty</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ford F-150 XLT</t>
+          <t>HVAC System #7375</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023 pickup truck, white, extended cab</t>
+          <t>Commercial HVAC unit</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Vehicles</t>
+          <t>Building Equipment</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2023-07-01</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>52000</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>15000</v>
+          <t>2021-02-03</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>14449.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>985.63</v>
       </c>
       <c r="G12" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Fleet vehicle #7 - Field service</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Toyota Camry LE</t>
+          <t>Printer #9818</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022 sedan, silver, company car</t>
+          <t>HP LaserJet multifunction printer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Vehicles</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2022-04-15</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>28500</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>8000</v>
+          <t>2020-05-06</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2414.09</v>
+      </c>
+      <c r="F13" t="n">
+        <v>309.28</v>
       </c>
       <c r="G13" t="n">
         <v>5</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Sales team vehicle</t>
+          <t>Refurbished</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chevrolet Express 2500</t>
+          <t>Conference Table #7785</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023 cargo van for deliveries</t>
+          <t>10-seat conference room table</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Vehicles</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023-09-10</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>38000</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>10000</v>
+          <t>2022-01-08</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>713.1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>61.62</v>
       </c>
       <c r="G14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Warehouse logistics</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tesla Model 3</t>
+          <t>Forklift #3865</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024 Long Range, blue, executive vehicle</t>
+          <t>Toyota electric forklift</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1033,571 +1003,567 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-01-05</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>47990</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>18000</v>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>49565.89</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4095.96</v>
       </c>
       <c r="G15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>CFO company car</t>
+          <t>Needs maintenance</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CNC Milling Machine</t>
+          <t>Office Desk #6372</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Haas VF-2 vertical machining center</t>
+          <t>Wooden executive office desk</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021-11-01</t>
-        </is>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>65000</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>8000</v>
+          <t>2025-11-17</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2310.94</v>
+      </c>
+      <c r="F16" t="n">
+        <v>273.49</v>
       </c>
       <c r="G16" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Production floor - Station 3</t>
+          <t>Extended warranty</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Industrial Air Compressor</t>
+          <t>Server Rack #4629</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ingersoll Rand 80-gallon, 7.5HP</t>
+          <t>Dell PowerEdge server</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2022-08-22</t>
-        </is>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>4500</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>400</v>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1469.21</v>
+      </c>
+      <c r="F17" t="n">
+        <v>116.82</v>
       </c>
       <c r="G17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>7-year property</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Maintenance shop</t>
-        </is>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Forklift - Electric</t>
+          <t>Company Car #1919</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Toyota 8FBCU25 5000lb capacity</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
-        </is>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>32000</v>
-      </c>
-      <c r="F18" s="1" t="n">
-        <v>5000</v>
+          <t>2017-10-24</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>67128.99000000001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>5211.68</v>
       </c>
       <c r="G18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Warehouse A</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Laser Cutter</t>
+          <t>Network Switch #4028</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Epilog Fusion Pro 48, 120W CO2</t>
+          <t>Cisco managed network switch</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-03-01</t>
-        </is>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>24995</v>
-      </c>
-      <c r="F19" s="1" t="n">
-        <v>2000</v>
+          <t>2018-06-29</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>3351.43</v>
+      </c>
+      <c r="F19" t="n">
+        <v>184.98</v>
       </c>
       <c r="G19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Prototyping lab</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3D Printer - Industrial</t>
+          <t>Network Switch #5379</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Stratasys F370, FDM technology</t>
+          <t>Cisco managed network switch</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023-06-18</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>18500</v>
-      </c>
-      <c r="F20" s="1" t="n">
-        <v>1500</v>
+          <t>2023-02-01</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1220.83</v>
+      </c>
+      <c r="F20" t="n">
+        <v>125.63</v>
       </c>
       <c r="G20" t="n">
         <v>5</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>R&amp;D department</t>
+          <t>Refurbished</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Warehouse Expansion</t>
+          <t>Backup Generator #5574</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5000 sq ft addition to east warehouse</t>
+          <t>Diesel backup generator</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Building Improvements</t>
+          <t>Building Equipment</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2022-05-01</t>
-        </is>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>450000</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>50000</v>
+          <t>2023-12-30</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>20574</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2404.05</v>
       </c>
       <c r="G21" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>39-year property</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Phase 2 expansion project</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>HVAC System Upgrade</t>
+          <t>Ergonomic Chair #1023</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Commercial rooftop units, building A</t>
+          <t>Herman Miller Aeron chair</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Building Improvements</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023-10-15</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>85000</v>
-      </c>
-      <c r="F22" s="1" t="n">
-        <v>5000</v>
+          <t>2018-03-10</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>1132.08</v>
+      </c>
+      <c r="F22" t="n">
+        <v>117.72</v>
       </c>
       <c r="G22" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>15-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Energy efficiency upgrade</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Parking Lot Repaving</t>
+          <t>Office Desk #6775</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Complete resurfacing with new striping</t>
+          <t>Wooden executive office desk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Land Improvements</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2023-04-20</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>35000</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>0</v>
+          <t>2016-12-11</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>214.21</v>
+      </c>
+      <c r="F23" t="n">
+        <v>15.43</v>
       </c>
       <c r="G23" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>15-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Front lot - 50 spaces</t>
+          <t>Refurbished</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Security System</t>
+          <t>Dell Laptop #9194</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>IP camera system with 32 cameras, NVR</t>
+          <t>Dell Latitude laptop computer</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Building Improvements</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-01-20</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>18500</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>1000</v>
+          <t>2020-01-27</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2842.24</v>
+      </c>
+      <c r="F24" t="n">
+        <v>233.65</v>
       </c>
       <c r="G24" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Facility-wide coverage</t>
+          <t>Extended warranty</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ERP System License</t>
+          <t>Server Rack #7702</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SAP Business One perpetual license</t>
+          <t>Dell PowerEdge server</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
-        </is>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>45000</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>0</v>
+          <t>2017-09-08</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>4632.37</v>
+      </c>
+      <c r="F25" t="n">
+        <v>602.8099999999999</v>
       </c>
       <c r="G25" t="n">
         <v>5</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Enterprise software - 25 users</t>
+          <t>Needs maintenance</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CAD Software Suite</t>
+          <t>Company Car #2943</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>AutoCAD + Inventor Professional</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2023-07-15</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="n">
-        <v>8500</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>0</v>
+          <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>52180.28</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5619.71</v>
       </c>
       <c r="G26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Engineering department</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CRM Platform</t>
+          <t>Company Car #5457</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Salesforce Enterprise - perpetual equivalent</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Software</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
-        </is>
-      </c>
-      <c r="E27" s="1" t="n">
-        <v>12000</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>0</v>
+          <t>2019-05-04</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>17923.18</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1636.79</v>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Sales and marketing</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Server Rack System</t>
+          <t>Company Car #1224</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Dell PowerEdge R750, dual Xeon, 256GB</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Computer Equipment</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
-        </is>
-      </c>
-      <c r="E28" s="1" t="n">
-        <v>18500</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>1000</v>
+          <t>2024-10-27</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>46223.3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3431.36</v>
       </c>
       <c r="G28" t="n">
         <v>5</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Primary application server</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>UPS Battery Backup</t>
+          <t>MacBook Pro #4333</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>APC Smart-UPS 5000VA rack-mount</t>
+          <t>Apple MacBook Pro 16-inch</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1607,38 +1573,38 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
-        </is>
-      </c>
-      <c r="E29" s="1" t="n">
-        <v>4200</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>200</v>
+          <t>2024-06-28</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>2566.07</v>
+      </c>
+      <c r="F29" t="n">
+        <v>351.07</v>
       </c>
       <c r="G29" t="n">
         <v>5</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Server room power backup</t>
+          <t>New purchase</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Network Switch Stack</t>
+          <t>Projector #3531</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cisco Catalyst 9300 48-port PoE+, qty 3</t>
+          <t>Epson business projector</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1648,274 +1614,865 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2023-06-01</t>
-        </is>
-      </c>
-      <c r="E30" s="1" t="n">
-        <v>15600</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <v>800</v>
+          <t>2016-09-06</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>3807.42</v>
+      </c>
+      <c r="F30" t="n">
+        <v>395.6</v>
       </c>
       <c r="G30" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Core network infrastructure</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Video Conference System</t>
+          <t>Forklift #8809</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Poly Studio X70 with TC8 controller</t>
+          <t>Toyota electric forklift</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Office Equipment</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2024-02-01</t>
-        </is>
-      </c>
-      <c r="E31" s="1" t="n">
-        <v>6500</v>
-      </c>
-      <c r="F31" s="1" t="n">
-        <v>300</v>
+          <t>2017-12-10</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>41653.58</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4851.71</v>
       </c>
       <c r="G31" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Executive conference room</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Commercial Generator</t>
+          <t>Ergonomic Chair #1697</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Generac 150kW natural gas standby</t>
+          <t>Herman Miller Aeron chair</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2022-12-10</t>
-        </is>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>42000</v>
-      </c>
-      <c r="F32" s="1" t="n">
-        <v>4000</v>
+          <t>2016-01-24</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1305.41</v>
+      </c>
+      <c r="F32" t="n">
+        <v>124.34</v>
       </c>
       <c r="G32" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>15-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Emergency backup power</t>
+          <t>Good condition</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Walk-in Cooler</t>
+          <t>Company Car #6690</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>8x10 commercial refrigeration unit</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Machinery</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2021-07-25</t>
-        </is>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>12500</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>1000</v>
+          <t>2025-11-03</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>54657.08</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5921.16</v>
       </c>
       <c r="G33" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>7-year property</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Break room storage</t>
-        </is>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Pallet Racking System</t>
+          <t>Printer #5375</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Heavy-duty warehouse shelving, 40 bays</t>
+          <t>HP LaserJet multifunction printer</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Furniture</t>
+          <t>Computer Equipment</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
-        </is>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>28000</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>3000</v>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>4777.07</v>
+      </c>
+      <c r="F34" t="n">
+        <v>671.77</v>
       </c>
       <c r="G34" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>7-year property</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Warehouse B storage</t>
+          <t>Extended warranty</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Office Renovation</t>
+          <t>Bookshelf #9477</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Complete remodel of 2nd floor offices</t>
+          <t>6-shelf office bookcase</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Building Improvements</t>
+          <t>Office Furniture</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
-        </is>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>125000</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>10000</v>
+          <t>2022-12-04</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>498.52</v>
+      </c>
+      <c r="F35" t="n">
+        <v>54.35</v>
       </c>
       <c r="G35" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>15-year property</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Executive suite upgrade</t>
+          <t>Refurbished</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Solar Panel Array</t>
+          <t>Company Car #8480</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>50kW rooftop solar installation</t>
+          <t>Toyota Camry sedan</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Building Improvements</t>
+          <t>Vehicles</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2024-04-01</t>
-        </is>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>95000</v>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>5000</v>
+          <t>2022-01-17</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>40031.52</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4256.7</v>
       </c>
       <c r="G36" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>5-year property</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Green energy initiative - ITC eligible</t>
-        </is>
-      </c>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Network Switch #6999</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Cisco managed network switch</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2023-03-30</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>3846.12</v>
+      </c>
+      <c r="F37" t="n">
+        <v>194.14</v>
+      </c>
+      <c r="G37" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>New purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Lathe #7654</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Industrial metal lathe</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Machinery</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2017-01-31</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>108804.65</v>
+      </c>
+      <c r="F38" t="n">
+        <v>11149.32</v>
+      </c>
+      <c r="G38" t="n">
+        <v>10</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Extended warranty</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Delivery Van #1527</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Ford Transit cargo van</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Vehicles</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2019-10-19</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>18754.65</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1664.49</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Good condition</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Server Rack #9384</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dell PowerEdge server</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2020-09-27</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>3427.6</v>
+      </c>
+      <c r="F40" t="n">
+        <v>175.08</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Extended warranty</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Projector #2753</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Epson business projector</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2023-09-05</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>2744.18</v>
+      </c>
+      <c r="F41" t="n">
+        <v>407.46</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Good condition</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Network Switch #4035</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Cisco managed network switch</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2019-03-11</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>642.36</v>
+      </c>
+      <c r="F42" t="n">
+        <v>62.31</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>New purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Projector #7525</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Epson business projector</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2017-01-08</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>1998.91</v>
+      </c>
+      <c r="F43" t="n">
+        <v>149.18</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>New purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Backup Generator #7386</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Diesel backup generator</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Building Equipment</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2024-06-22</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>23395.94</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2022.7</v>
+      </c>
+      <c r="G44" t="n">
+        <v>10</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Extended warranty</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Reception Desk #8814</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>L-shaped reception counter</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Office Furniture</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2024-02-29</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>2870.31</v>
+      </c>
+      <c r="F45" t="n">
+        <v>404.89</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Lathe #3348</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Industrial metal lathe</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Machinery</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>12814.25</v>
+      </c>
+      <c r="F46" t="n">
+        <v>892.13</v>
+      </c>
+      <c r="G46" t="n">
+        <v>10</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>New purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CNC Machine #7522</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Haas CNC milling machine</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Machinery</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>67080.34</v>
+      </c>
+      <c r="F47" t="n">
+        <v>7466.82</v>
+      </c>
+      <c r="G47" t="n">
+        <v>10</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Printer #4739</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>HP LaserJet multifunction printer</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2021-04-17</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>1981.86</v>
+      </c>
+      <c r="F48" t="n">
+        <v>265.95</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>HVAC System #2458</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Commercial HVAC unit</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Building Equipment</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2016-04-16</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>15985.57</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1646.59</v>
+      </c>
+      <c r="G49" t="n">
+        <v>15</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>New purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Lathe #4648</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Industrial metal lathe</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Machinery</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2022-08-05</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>88986.35000000001</v>
+      </c>
+      <c r="F50" t="n">
+        <v>10281.84</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Needs maintenance</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Dell Laptop #9917</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Dell Latitude laptop computer</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Computer Equipment</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2016-03-16</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>4316.68</v>
+      </c>
+      <c r="F51" t="n">
+        <v>557.46</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>